<commit_message>
Created script for county-cohort data; amended data structure for years in dataset; highlighted particularly bad hurricanes in Table 1
</commit_message>
<xml_diff>
--- a/data/data_structure_example/data structure example 2022 11 01.xlsx
+++ b/data/data_structure_example/data structure example 2022 11 01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/tropical_cyclones_educational_attainment_2022/data/data_structure_example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellameltzer/Git/tropical_cyclones_educational_attainment_2022/data/data_structure_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FF39F8-CC0B-2741-A16C-8148DD3A630C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B0DEDC-2EB6-474B-B4AF-CD128EF5BDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{30081CEF-72F0-214F-81A9-65715FEB61B2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{30081CEF-72F0-214F-81A9-65715FEB61B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="15">
   <si>
     <t>Covariates…</t>
   </si>
@@ -84,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,6 +105,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +169,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,11 +484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF57E9F-8B1C-594F-93E7-9B4D7D695C3F}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K116" sqref="K116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,7 +538,7 @@
         <v>A3</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2009</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -539,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f>F2*G2</f>
+        <f t="shared" ref="H2:H33" si="1">F2*G2</f>
         <v>0</v>
       </c>
       <c r="I2" t="s">
@@ -562,7 +573,7 @@
         <v>A3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>2010</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -574,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f>F3*G3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -597,7 +608,7 @@
         <v>A3</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2011</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -609,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <f>F4*G4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I4" t="s">
@@ -632,7 +643,7 @@
         <v>A3</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2012</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -644,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <f>F5*G5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I5" t="s">
@@ -663,7 +674,7 @@
         <v>A3</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>2013</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -675,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <f>F6*G6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I6" t="s">
@@ -694,7 +705,7 @@
         <v>A3</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>2014</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -706,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <f>F7*G7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I7" t="s">
@@ -718,14 +729,14 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>A4</v>
+        <v>A3</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -737,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f>F8*G8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" t="s">
@@ -749,14 +760,14 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>A4</v>
+        <v>A3</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>2016</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -768,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <f>F9*G9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" t="s">
@@ -780,14 +791,14 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>A4</v>
+        <v>A3</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2017</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -799,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <f>F10*G10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I10" t="s">
@@ -811,14 +822,14 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>A4</v>
+        <v>A3</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2018</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -830,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <f>F11*G11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I11" t="s">
@@ -849,7 +860,7 @@
         <v>A4</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2009</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -861,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <f>F12*G12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I12" t="s">
@@ -880,7 +891,7 @@
         <v>A4</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>2010</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
@@ -892,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <f>F13*G13</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I13" t="s">
@@ -904,14 +915,14 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>A5</v>
+        <v>A4</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2011</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -923,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <f>F14*G14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I14" t="s">
@@ -935,14 +946,14 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>A5</v>
+        <v>A4</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>2012</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -954,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <f>F15*G15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I15" t="s">
@@ -966,14 +977,14 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>A5</v>
+        <v>A4</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2013</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -985,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <f>F16*G16</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I16" t="s">
@@ -997,14 +1008,14 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>A5</v>
+        <v>A4</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2014</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -1016,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <f>F17*G17</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I17" t="s">
@@ -1028,14 +1039,14 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>A5</v>
+        <v>A4</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>2015</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
@@ -1047,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <f>F18*G18</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I18" t="s">
@@ -1059,14 +1070,14 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>A5</v>
+        <v>A4</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>2016</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
@@ -1078,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <f>F19*G19</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I19" t="s">
@@ -1090,14 +1101,14 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>A6</v>
+        <v>A4</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2017</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -1109,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f>F20*G20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I20" t="s">
@@ -1121,14 +1132,14 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>A6</v>
+        <v>A4</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>2018</v>
       </c>
       <c r="E21" t="s">
         <v>2</v>
@@ -1140,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <f>F21*G21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I21" t="s">
@@ -1152,14 +1163,14 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>A6</v>
+        <v>A5</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>2009</v>
       </c>
       <c r="E22" t="s">
         <v>2</v>
@@ -1171,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <f>F22*G22</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I22" t="s">
@@ -1183,14 +1194,14 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>A6</v>
+        <v>A5</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>2010</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
@@ -1202,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <f>F23*G23</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I23" t="s">
@@ -1214,14 +1225,14 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>A6</v>
+        <v>A5</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>2011</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
@@ -1233,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <f>F24*G24</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I24" t="s">
@@ -1245,14 +1256,14 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>A6</v>
+        <v>A5</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>2012</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
@@ -1264,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <f>F25*G25</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I25" t="s">
@@ -1276,14 +1287,14 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>A7</v>
+        <v>A5</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="E26" t="s">
         <v>2</v>
@@ -1295,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <f>F26*G26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I26" t="s">
@@ -1307,14 +1318,14 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>A7</v>
+        <v>A5</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>2014</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
@@ -1326,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <f>F27*G27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I27" t="s">
@@ -1338,14 +1349,14 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>A7</v>
+        <v>A5</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>2015</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
@@ -1357,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <f>F28*G28</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I28" t="s">
@@ -1369,14 +1380,14 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>A7</v>
+        <v>A5</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>2016</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
@@ -1388,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <f>F29*G29</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I29" t="s">
@@ -1400,14 +1411,14 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>A7</v>
+        <v>A5</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>2017</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
@@ -1419,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <f>F30*G30</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I30" t="s">
@@ -1431,14 +1442,14 @@
         <v>1</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>A7</v>
+        <v>A5</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>2018</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
@@ -1450,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <f>F31*G31</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I31" t="s">
@@ -1462,14 +1473,14 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>A8</v>
+        <v>A6</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2009</v>
       </c>
       <c r="E32" t="s">
         <v>2</v>
@@ -1481,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <f>F32*G32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I32" t="s">
@@ -1493,14 +1504,14 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>A8</v>
+        <v>A6</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>2010</v>
       </c>
       <c r="E33" t="s">
         <v>2</v>
@@ -1512,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <f>F33*G33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I33" t="s">
@@ -1524,14 +1535,14 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>A8</v>
+        <v>A6</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>2011</v>
       </c>
       <c r="E34" t="s">
         <v>2</v>
@@ -1543,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <f>F34*G34</f>
+        <f t="shared" ref="H34:H65" si="2">F34*G34</f>
         <v>1</v>
       </c>
       <c r="I34" t="s">
@@ -1555,14 +1566,14 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>A8</v>
+        <v>A6</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>2012</v>
       </c>
       <c r="E35" t="s">
         <v>2</v>
@@ -1574,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <f>F35*G35</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I35" t="s">
@@ -1586,14 +1597,14 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>A8</v>
+        <v>A6</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>2013</v>
       </c>
       <c r="E36" t="s">
         <v>2</v>
@@ -1605,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <f>F36*G36</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I36" t="s">
@@ -1617,14 +1628,14 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>A8</v>
+        <v>A6</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>2014</v>
       </c>
       <c r="E37" t="s">
         <v>2</v>
@@ -1636,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <f>F37*G37</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I37" t="s">
@@ -1648,14 +1659,14 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" ref="C38:C73" si="1">_xlfn.CONCAT(A38,B38)</f>
-        <v>B3</v>
+        <f t="shared" ref="C38:C101" si="3">_xlfn.CONCAT(A38,B38)</f>
+        <v>B6</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
@@ -1667,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <f>F38*G38</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I38" t="s">
@@ -1679,14 +1690,14 @@
         <v>3</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="1"/>
-        <v>B3</v>
+        <f t="shared" si="3"/>
+        <v>B6</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>2016</v>
       </c>
       <c r="E39" t="s">
         <v>2</v>
@@ -1698,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <f>F39*G39</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I39" t="s">
@@ -1710,14 +1721,14 @@
         <v>3</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="1"/>
-        <v>B3</v>
+        <f t="shared" si="3"/>
+        <v>B6</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>2017</v>
       </c>
       <c r="E40" t="s">
         <v>2</v>
@@ -1729,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <f>F40*G40</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I40" t="s">
@@ -1741,14 +1752,14 @@
         <v>3</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="1"/>
-        <v>B3</v>
+        <f t="shared" si="3"/>
+        <v>B6</v>
       </c>
       <c r="D41">
-        <v>4</v>
+        <v>2018</v>
       </c>
       <c r="E41" t="s">
         <v>2</v>
@@ -1760,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <f>F41*G41</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I41" t="s">
@@ -1772,14 +1783,14 @@
         <v>3</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="1"/>
-        <v>B3</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>2009</v>
       </c>
       <c r="E42" t="s">
         <v>2</v>
@@ -1791,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <f>F42*G42</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I42" t="s">
@@ -1803,14 +1814,14 @@
         <v>3</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="1"/>
-        <v>B3</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D43">
-        <v>6</v>
+        <v>2010</v>
       </c>
       <c r="E43" t="s">
         <v>2</v>
@@ -1822,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <f>F43*G43</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I43" t="s">
@@ -1834,14 +1845,14 @@
         <v>3</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="1"/>
-        <v>B4</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2011</v>
       </c>
       <c r="E44" t="s">
         <v>2</v>
@@ -1853,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <f>F44*G44</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I44" t="s">
@@ -1865,14 +1876,14 @@
         <v>3</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="1"/>
-        <v>B4</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>2012</v>
       </c>
       <c r="E45" t="s">
         <v>2</v>
@@ -1884,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <f>F45*G45</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I45" t="s">
@@ -1896,14 +1907,14 @@
         <v>3</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="1"/>
-        <v>B4</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>2013</v>
       </c>
       <c r="E46" t="s">
         <v>2</v>
@@ -1915,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <f>F46*G46</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I46" t="s">
@@ -1927,14 +1938,14 @@
         <v>3</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="1"/>
-        <v>B4</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>2014</v>
       </c>
       <c r="E47" t="s">
         <v>2</v>
@@ -1946,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="H47">
-        <f>F47*G47</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I47" t="s">
@@ -1958,14 +1969,14 @@
         <v>3</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="1"/>
-        <v>B4</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>2015</v>
       </c>
       <c r="E48" t="s">
         <v>2</v>
@@ -1977,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="H48">
-        <f>F48*G48</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I48" t="s">
@@ -1989,14 +2000,14 @@
         <v>3</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="1"/>
-        <v>B4</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>2016</v>
       </c>
       <c r="E49" t="s">
         <v>2</v>
@@ -2008,7 +2019,7 @@
         <v>1</v>
       </c>
       <c r="H49">
-        <f>F49*G49</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I49" t="s">
@@ -2020,14 +2031,14 @@
         <v>3</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="1"/>
-        <v>B5</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>2017</v>
       </c>
       <c r="E50" t="s">
         <v>2</v>
@@ -2039,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="H50">
-        <f>F50*G50</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I50" t="s">
@@ -2051,14 +2062,14 @@
         <v>3</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="1"/>
-        <v>B5</v>
+        <f t="shared" si="3"/>
+        <v>B7</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>2018</v>
       </c>
       <c r="E51" t="s">
         <v>2</v>
@@ -2070,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <f>F51*G51</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I51" t="s">
@@ -2082,14 +2093,14 @@
         <v>3</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C52" t="str">
-        <f t="shared" si="1"/>
-        <v>B5</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>2009</v>
       </c>
       <c r="E52" t="s">
         <v>2</v>
@@ -2101,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="H52">
-        <f>F52*G52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I52" t="s">
@@ -2113,14 +2124,14 @@
         <v>3</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C53" t="str">
-        <f t="shared" si="1"/>
-        <v>B5</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>2010</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
@@ -2132,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <f>F53*G53</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I53" t="s">
@@ -2144,14 +2155,14 @@
         <v>3</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C54" t="str">
-        <f t="shared" si="1"/>
-        <v>B5</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>2011</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
@@ -2163,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="H54">
-        <f>F54*G54</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I54" t="s">
@@ -2175,14 +2186,14 @@
         <v>3</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C55" t="str">
-        <f t="shared" si="1"/>
-        <v>B5</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D55">
-        <v>6</v>
+        <v>2012</v>
       </c>
       <c r="E55" t="s">
         <v>2</v>
@@ -2194,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="H55">
-        <f>F55*G55</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I55" t="s">
@@ -2206,14 +2217,14 @@
         <v>3</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" si="1"/>
-        <v>B6</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="E56" t="s">
         <v>2</v>
@@ -2225,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <f>F56*G56</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I56" t="s">
@@ -2237,14 +2248,14 @@
         <v>3</v>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C57" t="str">
-        <f t="shared" si="1"/>
-        <v>B6</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>2014</v>
       </c>
       <c r="E57" t="s">
         <v>2</v>
@@ -2256,7 +2267,7 @@
         <v>0</v>
       </c>
       <c r="H57">
-        <f>F57*G57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I57" t="s">
@@ -2268,14 +2279,14 @@
         <v>3</v>
       </c>
       <c r="B58">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C58" t="str">
-        <f t="shared" si="1"/>
-        <v>B6</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>2015</v>
       </c>
       <c r="E58" t="s">
         <v>2</v>
@@ -2287,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="H58">
-        <f>F58*G58</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I58" t="s">
@@ -2299,14 +2310,14 @@
         <v>3</v>
       </c>
       <c r="B59">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C59" t="str">
-        <f t="shared" si="1"/>
-        <v>B6</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>2016</v>
       </c>
       <c r="E59" t="s">
         <v>2</v>
@@ -2318,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="H59">
-        <f>F59*G59</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I59" t="s">
@@ -2330,14 +2341,14 @@
         <v>3</v>
       </c>
       <c r="B60">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60" t="str">
-        <f t="shared" si="1"/>
-        <v>B6</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D60">
-        <v>5</v>
+        <v>2017</v>
       </c>
       <c r="E60" t="s">
         <v>2</v>
@@ -2349,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="H60">
-        <f>F60*G60</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I60" t="s">
@@ -2361,14 +2372,14 @@
         <v>3</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C61" t="str">
-        <f t="shared" si="1"/>
-        <v>B6</v>
+        <f t="shared" si="3"/>
+        <v>B8</v>
       </c>
       <c r="D61">
-        <v>6</v>
+        <v>2018</v>
       </c>
       <c r="E61" t="s">
         <v>2</v>
@@ -2380,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="H61">
-        <f>F61*G61</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I61" t="s">
@@ -2392,14 +2403,14 @@
         <v>3</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C62" t="str">
-        <f t="shared" si="1"/>
-        <v>B7</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>2009</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
@@ -2411,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <f>F62*G62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I62" t="s">
@@ -2423,14 +2434,14 @@
         <v>3</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C63" t="str">
-        <f t="shared" si="1"/>
-        <v>B7</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>2010</v>
       </c>
       <c r="E63" t="s">
         <v>2</v>
@@ -2442,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <f>F63*G63</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I63" t="s">
@@ -2454,14 +2465,14 @@
         <v>3</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C64" t="str">
-        <f t="shared" si="1"/>
-        <v>B7</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>2011</v>
       </c>
       <c r="E64" t="s">
         <v>2</v>
@@ -2473,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="H64">
-        <f>F64*G64</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I64" t="s">
@@ -2485,14 +2496,14 @@
         <v>3</v>
       </c>
       <c r="B65">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C65" t="str">
-        <f t="shared" si="1"/>
-        <v>B7</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>2012</v>
       </c>
       <c r="E65" t="s">
         <v>2</v>
@@ -2504,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <f>F65*G65</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I65" t="s">
@@ -2516,14 +2527,14 @@
         <v>3</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" si="1"/>
-        <v>B7</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D66">
-        <v>5</v>
+        <v>2013</v>
       </c>
       <c r="E66" t="s">
         <v>2</v>
@@ -2535,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <f>F66*G66</f>
+        <f t="shared" ref="H66:H121" si="4">F66*G66</f>
         <v>0</v>
       </c>
       <c r="I66" t="s">
@@ -2547,14 +2558,14 @@
         <v>3</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v>B7</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D67">
-        <v>6</v>
+        <v>2014</v>
       </c>
       <c r="E67" t="s">
         <v>2</v>
@@ -2566,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <f>F67*G67</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I67" t="s">
@@ -2578,14 +2589,14 @@
         <v>3</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C68" t="str">
-        <f t="shared" si="1"/>
-        <v>B8</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="E68" t="s">
         <v>2</v>
@@ -2597,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <f>F68*G68</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I68" t="s">
@@ -2609,14 +2620,14 @@
         <v>3</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C69" t="str">
-        <f t="shared" si="1"/>
-        <v>B8</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>2016</v>
       </c>
       <c r="E69" t="s">
         <v>2</v>
@@ -2628,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="H69">
-        <f>F69*G69</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I69" t="s">
@@ -2640,14 +2651,14 @@
         <v>3</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="1"/>
-        <v>B8</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>2017</v>
       </c>
       <c r="E70" t="s">
         <v>2</v>
@@ -2659,7 +2670,7 @@
         <v>1</v>
       </c>
       <c r="H70">
-        <f>F70*G70</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I70" t="s">
@@ -2671,14 +2682,14 @@
         <v>3</v>
       </c>
       <c r="B71">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C71" t="str">
-        <f t="shared" si="1"/>
-        <v>B8</v>
+        <f t="shared" si="3"/>
+        <v>B3</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>2018</v>
       </c>
       <c r="E71" t="s">
         <v>2</v>
@@ -2690,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="H71">
-        <f>F71*G71</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I71" t="s">
@@ -2702,14 +2713,14 @@
         <v>3</v>
       </c>
       <c r="B72">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C72" t="str">
-        <f t="shared" si="1"/>
-        <v>B8</v>
+        <f t="shared" si="3"/>
+        <v>B4</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>2009</v>
       </c>
       <c r="E72" t="s">
         <v>2</v>
@@ -2721,7 +2732,7 @@
         <v>1</v>
       </c>
       <c r="H72">
-        <f>F72*G72</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I72" t="s">
@@ -2733,29 +2744,1517 @@
         <v>3</v>
       </c>
       <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D73">
+        <v>2010</v>
+      </c>
+      <c r="E73" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D74">
+        <v>2011</v>
+      </c>
+      <c r="E74" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D75">
+        <v>2012</v>
+      </c>
+      <c r="E75" t="s">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D76">
+        <v>2013</v>
+      </c>
+      <c r="E76" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D77">
+        <v>2014</v>
+      </c>
+      <c r="E77" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D78">
+        <v>2015</v>
+      </c>
+      <c r="E78" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D79">
+        <v>2016</v>
+      </c>
+      <c r="E79" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D80">
+        <v>2017</v>
+      </c>
+      <c r="E80" t="s">
+        <v>2</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="3"/>
+        <v>B4</v>
+      </c>
+      <c r="D81">
+        <v>2018</v>
+      </c>
+      <c r="E81" t="s">
+        <v>2</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D82" s="5">
+        <v>2009</v>
+      </c>
+      <c r="E82" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D83" s="5">
+        <v>2010</v>
+      </c>
+      <c r="E83" t="s">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D84" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E84" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D85" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E85" t="s">
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D86" s="5">
+        <v>2013</v>
+      </c>
+      <c r="E86" t="s">
+        <v>2</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D87" s="5">
+        <v>2014</v>
+      </c>
+      <c r="E87" t="s">
+        <v>2</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D88" s="5">
+        <v>2015</v>
+      </c>
+      <c r="E88" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>5</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D89" s="5">
+        <v>2016</v>
+      </c>
+      <c r="E89" t="s">
+        <v>2</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D90" s="5">
+        <v>2017</v>
+      </c>
+      <c r="E90" t="s">
+        <v>2</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="3"/>
+        <v>B5</v>
+      </c>
+      <c r="D91" s="5">
+        <v>2018</v>
+      </c>
+      <c r="E91" t="s">
+        <v>2</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <v>6</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D92" s="5">
+        <v>2009</v>
+      </c>
+      <c r="E92" t="s">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93">
+        <v>6</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D93" s="5">
+        <v>2010</v>
+      </c>
+      <c r="E93" t="s">
+        <v>2</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>6</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D94" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E94" t="s">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>6</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D95" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E95" t="s">
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96">
+        <v>6</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D96" s="5">
+        <v>2013</v>
+      </c>
+      <c r="E96" t="s">
+        <v>2</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97">
+        <v>6</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D97" s="5">
+        <v>2014</v>
+      </c>
+      <c r="E97" t="s">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D98" s="5">
+        <v>2015</v>
+      </c>
+      <c r="E98" t="s">
+        <v>2</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99">
+        <v>6</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D99" s="5">
+        <v>2016</v>
+      </c>
+      <c r="E99" t="s">
+        <v>2</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100">
+        <v>6</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D100" s="5">
+        <v>2017</v>
+      </c>
+      <c r="E100" t="s">
+        <v>2</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101">
+        <v>6</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="3"/>
+        <v>B6</v>
+      </c>
+      <c r="D101" s="5">
+        <v>2018</v>
+      </c>
+      <c r="E101" t="s">
+        <v>2</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102">
+        <v>7</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" ref="C102:C121" si="5">_xlfn.CONCAT(A102,B102)</f>
+        <v>B7</v>
+      </c>
+      <c r="D102" s="5">
+        <v>2009</v>
+      </c>
+      <c r="E102" t="s">
+        <v>2</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>7</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2010</v>
+      </c>
+      <c r="E103" t="s">
+        <v>2</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>3</v>
+      </c>
+      <c r="B104">
+        <v>7</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D104" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E104" t="s">
+        <v>2</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105">
+        <v>7</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D105" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E105" t="s">
+        <v>2</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106">
+        <v>7</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D106" s="5">
+        <v>2013</v>
+      </c>
+      <c r="E106" t="s">
+        <v>2</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>7</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D107" s="5">
+        <v>2014</v>
+      </c>
+      <c r="E107" t="s">
+        <v>2</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108">
+        <v>7</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D108" s="5">
+        <v>2015</v>
+      </c>
+      <c r="E108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109">
+        <v>7</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D109" s="5">
+        <v>2016</v>
+      </c>
+      <c r="E109" t="s">
+        <v>2</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>1</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>7</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D110" s="5">
+        <v>2017</v>
+      </c>
+      <c r="E110" t="s">
+        <v>2</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>7</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="5"/>
+        <v>B7</v>
+      </c>
+      <c r="D111" s="5">
+        <v>2018</v>
+      </c>
+      <c r="E111" t="s">
+        <v>2</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112">
         <v>8</v>
       </c>
-      <c r="C73" t="str">
-        <f t="shared" si="1"/>
+      <c r="C112" t="str">
+        <f t="shared" si="5"/>
         <v>B8</v>
       </c>
-      <c r="D73">
-        <v>6</v>
-      </c>
-      <c r="E73" t="s">
-        <v>2</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
-      <c r="H73">
-        <f>F73*G73</f>
-        <v>0</v>
-      </c>
-      <c r="I73" t="s">
+      <c r="D112" s="5">
+        <v>2009</v>
+      </c>
+      <c r="E112" t="s">
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>1</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113">
+        <v>8</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D113" s="5">
+        <v>2010</v>
+      </c>
+      <c r="E113" t="s">
+        <v>2</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114">
+        <v>8</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D114" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E114" t="s">
+        <v>2</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115">
+        <v>8</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D115" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E115" t="s">
+        <v>2</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>1</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116">
+        <v>8</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D116" s="5">
+        <v>2013</v>
+      </c>
+      <c r="E116" t="s">
+        <v>2</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>3</v>
+      </c>
+      <c r="B117">
+        <v>8</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D117" s="5">
+        <v>2014</v>
+      </c>
+      <c r="E117" t="s">
+        <v>2</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <v>1</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D118" s="5">
+        <v>2015</v>
+      </c>
+      <c r="E118" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119">
+        <v>8</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D119" s="5">
+        <v>2016</v>
+      </c>
+      <c r="E119" t="s">
+        <v>2</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>1</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>8</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D120" s="5">
+        <v>2017</v>
+      </c>
+      <c r="E120" t="s">
+        <v>2</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>1</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>8</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="5"/>
+        <v>B8</v>
+      </c>
+      <c r="D121" s="5">
+        <v>2018</v>
+      </c>
+      <c r="E121" t="s">
+        <v>2</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I121" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added tropical cyclone exposure data for DID model
</commit_message>
<xml_diff>
--- a/data/data_structure_example/data structure example 2022 11 01.xlsx
+++ b/data/data_structure_example/data structure example 2022 11 01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellameltzer/Git/tropical_cyclones_educational_attainment_2022/data/data_structure_example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmiparks/git/tropical_cyclones_educational_attainment_2022/data/data_structure_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B0DEDC-2EB6-474B-B4AF-CD128EF5BDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53F58B5-D010-FF42-A534-5D1E644C48A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{30081CEF-72F0-214F-81A9-65715FEB61B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{30081CEF-72F0-214F-81A9-65715FEB61B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,49 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Robbie Parks</author>
+  </authors>
+  <commentList>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{FC53ED23-3EF2-D749-8086-65C2D5986183}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Robbie Parks:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella: Need to fix this as once exposed always epxposed in a coutny</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -87,7 +130,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +158,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -483,12 +539,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF57E9F-8B1C-594F-93E7-9B4D7D695C3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF57E9F-8B1C-594F-93E7-9B4D7D695C3F}">
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K116" sqref="K116"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4261,5 +4317,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>